<commit_message>
Added CCITT-2 overview sheet
</commit_message>
<xml_diff>
--- a/CCITT-2.xlsx
+++ b/CCITT-2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITHUB\piTelex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{73BE8221-DDE8-4362-B3C8-7D2ECE553CCA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D5C77892-75E5-4BF5-946E-AA64DB0C5724}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20790" windowHeight="11790" xr2:uid="{6A197C08-2C96-45F9-8B7D-250934CD9C78}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20790" windowHeight="11790" activeTab="1" xr2:uid="{6A197C08-2C96-45F9-8B7D-250934CD9C78}"/>
   </bookViews>
   <sheets>
     <sheet name="CCITT-2" sheetId="1" r:id="rId1"/>
@@ -502,12 +502,6 @@
     <t>P…</t>
   </si>
   <si>
-    <t>Kein Strom (A)</t>
-  </si>
-  <si>
-    <t>Strom (Z)</t>
-  </si>
-  <si>
     <t>Symbol</t>
   </si>
   <si>
@@ -622,6 +616,12 @@
   </si>
   <si>
     <t>Space</t>
+  </si>
+  <si>
+    <t>Stromschritt (Z) 40mA</t>
+  </si>
+  <si>
+    <t>Stoppschritt (A) 0mA</t>
   </si>
 </sst>
 </file>
@@ -1373,7 +1373,7 @@
   </sheetPr>
   <dimension ref="A1:AC36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AB20" sqref="AB20"/>
     </sheetView>
   </sheetViews>
@@ -1401,7 +1401,7 @@
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:29" s="34" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1422,14 +1422,14 @@
         <v>116</v>
       </c>
       <c r="G4" s="28" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H4" s="48"/>
       <c r="I4" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="J4" s="28" t="s">
         <v>136</v>
-      </c>
-      <c r="J4" s="28" t="s">
-        <v>138</v>
       </c>
       <c r="K4" s="48"/>
       <c r="L4" s="28" t="s">
@@ -1443,10 +1443,10 @@
       </c>
       <c r="O4" s="48"/>
       <c r="P4" s="28" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="Q4" s="28" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="R4" s="31"/>
       <c r="S4" s="28" t="s">
@@ -1639,7 +1639,7 @@
         <v>8</v>
       </c>
       <c r="Q7" s="61" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="R7" s="4"/>
       <c r="S7" s="12"/>
@@ -1926,7 +1926,7 @@
         <v>10</v>
       </c>
       <c r="J12" s="39" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="K12" s="43"/>
       <c r="L12" s="56" t="s">
@@ -2006,7 +2006,7 @@
         <v>11</v>
       </c>
       <c r="Q13" s="61" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="R13" s="4"/>
       <c r="S13" s="12"/>
@@ -2378,10 +2378,10 @@
       </c>
       <c r="O19" s="41"/>
       <c r="P19" s="60" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="Q19" s="60" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="R19" s="4"/>
       <c r="S19" s="12"/>
@@ -2814,7 +2814,7 @@
         <v>19</v>
       </c>
       <c r="Q26" s="61" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="R26" s="4"/>
       <c r="S26" s="12"/>
@@ -3007,7 +3007,7 @@
         <v>27</v>
       </c>
       <c r="Q29" s="61" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="R29" s="4"/>
       <c r="S29" s="12"/>
@@ -3249,7 +3249,7 @@
         <v>22</v>
       </c>
       <c r="Q33" s="65" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="R33" s="16"/>
       <c r="S33" s="12"/>
@@ -3474,8 +3474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1976E10-A211-4471-8DF6-ECC4CDD78CAC}">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3488,7 +3488,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="24" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
@@ -3496,7 +3496,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B4" s="23" t="s">
         <v>83</v>
@@ -3505,7 +3505,7 @@
         <v>82</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -3516,10 +3516,10 @@
         <v>67</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E5" s="67" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -3530,10 +3530,10 @@
         <v>70</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E6" s="67" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -3561,7 +3561,7 @@
         <v>79</v>
       </c>
       <c r="E8" s="67" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -3575,7 +3575,7 @@
         <v>80</v>
       </c>
       <c r="E9" s="68" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -3589,7 +3589,7 @@
         <v>81</v>
       </c>
       <c r="E10" s="68" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -3597,11 +3597,11 @@
         <v>120</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C11" s="14"/>
       <c r="E11" s="73" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -3612,7 +3612,7 @@
         <v>37</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E12" s="18" t="s">
         <v>65</v>
@@ -3626,19 +3626,19 @@
         <v>84</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E13" s="67" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="25" t="s">
-        <v>121</v>
+        <v>159</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -3646,72 +3646,72 @@
         <v>40</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>122</v>
+        <v>158</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="20"/>
       <c r="E20" s="70" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="20"/>
       <c r="E21" s="70" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="72" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E22" s="70" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="20" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E23" s="70" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="20"/>
       <c r="E24" s="70" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="72" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E25" s="70" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="72" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E26" s="70" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="20"/>
       <c r="E27" s="71" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="20"/>
       <c r="E28" s="71" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">

</xml_diff>